<commit_message>
Added database upload module
</commit_message>
<xml_diff>
--- a/Documents/SatelliteTimes.xlsx
+++ b/Documents/SatelliteTimes.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>Altimeter</t>
   </si>
@@ -222,12 +222,6 @@
   </si>
   <si>
     <t>&lt;90</t>
-  </si>
-  <si>
-    <t>Check</t>
-  </si>
-  <si>
-    <t>start and end dates</t>
   </si>
 </sst>
 </file>
@@ -568,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AM22"/>
+  <dimension ref="A1:AM16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -838,30 +832,30 @@
       <c r="AA6" s="1"/>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -1100,16 +1094,6 @@
       <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>67</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>